<commit_message>
[mnp] excel: drop down item with vlookup
</commit_message>
<xml_diff>
--- a/mnp/slg/skill_list_MAP.xlsx
+++ b/mnp/slg/skill_list_MAP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MinWee\Desktop\MAP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\map_docs\skills\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="183">
   <si>
     <t>sub_skill_id</t>
   </si>
@@ -74,9 +74,6 @@
     <t>HP</t>
   </si>
   <si>
-    <t>status_type</t>
-  </si>
-  <si>
     <t>Skill ID</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
   </si>
   <si>
     <t>Dark</t>
-  </si>
-  <si>
-    <t>Poison</t>
   </si>
   <si>
     <t>Silence</t>
@@ -364,9 +358,6 @@
     </r>
   </si>
   <si>
-    <t>Dispel</t>
-  </si>
-  <si>
     <t>Buff(ATK)</t>
   </si>
   <si>
@@ -473,9 +464,6 @@
     <t>None/ALL</t>
   </si>
   <si>
-    <t>Remove statuses</t>
-  </si>
-  <si>
     <t>Buff(Mana)</t>
   </si>
   <si>
@@ -576,9 +564,6 @@
     </r>
   </si>
   <si>
-    <t>Heal</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Target gains </t>
     </r>
@@ -729,49 +714,19 @@
     <t>Buff(Critical)</t>
   </si>
   <si>
-    <t>Apply to all Nature hero</t>
-  </si>
-  <si>
-    <t>Apply to all Ice hero</t>
-  </si>
-  <si>
-    <t>Apply to all Light hero</t>
-  </si>
-  <si>
-    <t>Apply to all Dark hero</t>
-  </si>
-  <si>
     <t>Buff(Accuracy)</t>
   </si>
   <si>
     <t>Lifesteal</t>
   </si>
   <si>
-    <t xml:space="preserve">Heal X% amount of Y damage dealt  </t>
-  </si>
-  <si>
     <t>Immune</t>
   </si>
   <si>
-    <t>Negative</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Neutral</t>
-  </si>
-  <si>
     <t>Shared Dmg</t>
   </si>
   <si>
     <t>Sub Skill ID</t>
-  </si>
-  <si>
-    <t>Sub Skill Name</t>
-  </si>
-  <si>
-    <t>Sub Skill Description</t>
   </si>
   <si>
     <t>Target type</t>
@@ -994,9 +949,6 @@
     </r>
   </si>
   <si>
-    <t>X Damage is shared</t>
-  </si>
-  <si>
     <t>para2</t>
   </si>
   <si>
@@ -1108,34 +1060,239 @@
     <t>turns</t>
   </si>
   <si>
-    <t>Fist Blast</t>
-  </si>
-  <si>
-    <t>Deal 225% damage to a target</t>
-  </si>
-  <si>
-    <t>asset_id</t>
-  </si>
-  <si>
-    <t>freeze</t>
-  </si>
-  <si>
-    <t>Target type description</t>
-  </si>
-  <si>
     <t>para12</t>
   </si>
   <si>
     <t>chc</t>
   </si>
   <si>
-    <t>Apply to all Fire hero</t>
-  </si>
-  <si>
     <t>chc_miss</t>
   </si>
   <si>
     <t>Chance to miss</t>
+  </si>
+  <si>
+    <t>Take Damage</t>
+  </si>
+  <si>
+    <t>Fire allies</t>
+  </si>
+  <si>
+    <t>Apply to all Fire allies</t>
+  </si>
+  <si>
+    <t>Nature allies</t>
+  </si>
+  <si>
+    <t>Apply to all Nature allies</t>
+  </si>
+  <si>
+    <t>Ice allies</t>
+  </si>
+  <si>
+    <t>Apply to all Ice allies</t>
+  </si>
+  <si>
+    <t>Light allies</t>
+  </si>
+  <si>
+    <t>Apply to all Light allies</t>
+  </si>
+  <si>
+    <t>Dark allies</t>
+  </si>
+  <si>
+    <t>Apply to all Dark allies</t>
+  </si>
+  <si>
+    <t>Fire enemies</t>
+  </si>
+  <si>
+    <t>Apply to all Fire enemies</t>
+  </si>
+  <si>
+    <t>Nature enemies</t>
+  </si>
+  <si>
+    <t>Apply to all Nature enemies</t>
+  </si>
+  <si>
+    <t>Ice enemies</t>
+  </si>
+  <si>
+    <t>Apply to all Ice enemies</t>
+  </si>
+  <si>
+    <t>Buff(HP)</t>
+  </si>
+  <si>
+    <t>Light enemies</t>
+  </si>
+  <si>
+    <t>Apply to all Light enemies</t>
+  </si>
+  <si>
+    <t>Dark enemies</t>
+  </si>
+  <si>
+    <t>Apply to all Dark enemies</t>
+  </si>
+  <si>
+    <t>Dispel(debuff)</t>
+  </si>
+  <si>
+    <t>Random ally</t>
+  </si>
+  <si>
+    <t>Apply to a random ally</t>
+  </si>
+  <si>
+    <t>Dispel(buff)</t>
+  </si>
+  <si>
+    <t>Random enemy</t>
+  </si>
+  <si>
+    <t>Apply to a random enemy</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Remove all debuff statuses</t>
+  </si>
+  <si>
+    <t>Remove all buff statuses</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Heal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> amount of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">damage dealt  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Damage is shared</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Charge up</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> X%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of break bar</t>
+    </r>
+  </si>
+  <si>
+    <t>Sub Skill Name(ref)</t>
+  </si>
+  <si>
+    <t>Sub Skill Description(ref)</t>
+  </si>
+  <si>
+    <t>Sub skill 2 description</t>
+  </si>
+  <si>
+    <t>Sub skill 3 description</t>
+  </si>
+  <si>
+    <t>Sub skill 4 description</t>
+  </si>
+  <si>
+    <t>Sub skill 5 description</t>
+  </si>
+  <si>
+    <t>Sub skill 1 description</t>
+  </si>
+  <si>
+    <t>Target type description(ref)</t>
+  </si>
+  <si>
+    <t>Value type description(ref)</t>
+  </si>
+  <si>
+    <t>FIELD TYPE</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>PERCENTAGE</t>
+  </si>
+  <si>
+    <t>PARAM1</t>
+  </si>
+  <si>
+    <t>PARAM2</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1431,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1321,6 +1478,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1606,18 +1766,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:O102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1" max="15" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="6">
         <v>0</v>
       </c>
@@ -1627,27 +1787,44 @@
       <c r="C1" s="6">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="6">
+        <v>3</v>
+      </c>
       <c r="E1" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6">
+        <v>13</v>
+      </c>
+      <c r="O1" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -1658,28 +1835,33 @@
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1690,8 +1872,13 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1702,60 +1889,77 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="G5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="I5" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="K5" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="M5" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1001</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>149</v>
-      </c>
+      <c r="O5" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>100002</v>
-      </c>
-      <c r="F6" s="2">
-        <v>100003</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1766,8 +1970,13 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1778,8 +1987,13 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1790,8 +2004,13 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1802,8 +2021,13 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1814,8 +2038,13 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1826,8 +2055,13 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1838,8 +2072,13 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1850,8 +2089,13 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1862,8 +2106,13 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1874,8 +2123,13 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1886,8 +2140,13 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1898,8 +2157,13 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1910,8 +2174,13 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1922,8 +2191,13 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1934,8 +2208,13 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1946,8 +2225,13 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1958,8 +2242,13 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1970,8 +2259,13 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1982,8 +2276,13 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1994,8 +2293,13 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2006,8 +2310,13 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2018,8 +2327,13 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2030,8 +2344,13 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2042,8 +2361,13 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2054,8 +2378,13 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2066,8 +2395,13 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2078,8 +2412,13 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2090,8 +2429,13 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2102,8 +2446,13 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2114,8 +2463,13 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2126,8 +2480,13 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2138,8 +2497,13 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2150,8 +2514,13 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2162,8 +2531,13 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2174,8 +2548,13 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2186,8 +2565,13 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2198,8 +2582,13 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2210,8 +2599,13 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2222,8 +2616,13 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2234,8 +2633,13 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2246,8 +2650,13 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2258,8 +2667,13 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2270,8 +2684,13 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2282,8 +2701,13 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2294,8 +2718,13 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2306,8 +2735,13 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2318,8 +2752,13 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2330,8 +2769,13 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2342,8 +2786,13 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2354,8 +2803,13 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2366,8 +2820,13 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2378,8 +2837,13 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2390,8 +2854,13 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2402,8 +2871,13 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2414,8 +2888,13 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2426,8 +2905,13 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2438,8 +2922,13 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2450,8 +2939,13 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2462,8 +2956,13 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2474,8 +2973,13 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2486,8 +2990,13 @@
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2498,8 +3007,13 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2510,8 +3024,13 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2522,8 +3041,13 @@
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2534,8 +3058,13 @@
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2546,8 +3075,13 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2558,8 +3092,13 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2570,8 +3109,13 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2582,8 +3126,13 @@
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2594,8 +3143,13 @@
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2606,8 +3160,13 @@
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2618,8 +3177,13 @@
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2630,8 +3194,13 @@
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" s="2"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2642,8 +3211,13 @@
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2654,8 +3228,13 @@
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2666,8 +3245,13 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="2"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2678,8 +3262,13 @@
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
+      <c r="O83" s="2"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2690,8 +3279,13 @@
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2702,8 +3296,13 @@
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2714,8 +3313,13 @@
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2726,8 +3330,13 @@
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2738,8 +3347,13 @@
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K88" s="2"/>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+      <c r="O88" s="2"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2750,8 +3364,13 @@
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="2"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2762,8 +3381,13 @@
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+      <c r="O90" s="2"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2774,8 +3398,13 @@
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="2"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2786,8 +3415,13 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2798,8 +3432,13 @@
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" s="2"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2810,8 +3449,13 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" s="2"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2822,8 +3466,13 @@
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2"/>
+      <c r="N95" s="2"/>
+      <c r="O95" s="2"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2834,8 +3483,13 @@
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2846,8 +3500,13 @@
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" s="2"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2858,8 +3517,13 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" s="2"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2870,8 +3534,13 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K99" s="2"/>
+      <c r="L99" s="2"/>
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
+      <c r="O99" s="2"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2882,8 +3551,13 @@
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
+      <c r="M100" s="2"/>
+      <c r="N100" s="2"/>
+      <c r="O100" s="2"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2894,8 +3568,13 @@
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+      <c r="O101" s="2"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2906,6 +3585,11 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2966,7 +3650,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>7</v>
@@ -2984,7 +3668,7 @@
         <v>11</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3013,34 +3697,34 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="J5" s="6" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4214,18 +4898,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="49" style="15" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="15" customWidth="1"/>
-    <col min="5" max="16" width="20.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="20.7109375" style="15" customWidth="1"/>
     <col min="17" max="17" width="20.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4239,9 +4925,7 @@
       <c r="C1" s="14">
         <v>2</v>
       </c>
-      <c r="D1" s="14">
-        <v>3</v>
-      </c>
+      <c r="D1" s="14"/>
       <c r="E1" s="14">
         <v>4</v>
       </c>
@@ -4287,65 +4971,63 @@
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>148</v>
-      </c>
+      <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>93</v>
+        <v>169</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>12</v>
@@ -4357,43 +5039,22 @@
         <v>14</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>100001</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>100002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>100003</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -4403,341 +5064,391 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V38"/>
+  <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.5703125" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K1" s="8" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>112</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="N1" s="8"/>
       <c r="O1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="P1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="U1" s="8" t="s">
+      <c r="AD1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="V1" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="R2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="V2" s="17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AD2" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
-      <c r="S4" s="12" t="s">
-        <v>117</v>
-      </c>
+      <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
-      <c r="S5" s="12" t="s">
-        <v>117</v>
-      </c>
+      <c r="S5" s="3"/>
       <c r="T5" s="3"/>
-      <c r="U5" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
-      <c r="S6" s="12"/>
+      <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3">
         <v>4</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -4745,152 +5456,160 @@
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3">
         <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -4898,269 +5617,302 @@
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>141</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>141</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U13" s="3"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="J14" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>97</v>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="12"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="12" t="s">
-        <v>117</v>
-      </c>
+      <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>3</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>16</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -5168,35 +5920,37 @@
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-      <c r="T19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>57</v>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>17</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -5205,260 +5959,677 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
-      <c r="U20" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>5</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J21" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
-      <c r="S21" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>0</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>3</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>5</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>6</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q29" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="3">
+        <v>100</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>8</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31" s="3">
+        <v>10</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>11</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>12</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>13</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>14</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="J37" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="K37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>15</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>16</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>17</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>18</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C41" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>19</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>8</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>9</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>10</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C42" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>20</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J44" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>11</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>12</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>13</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>14</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="K44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
+        <v>0</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J47" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>15</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>16</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>17</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>18</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="13">
-        <v>0</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="K47" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+    </row>
+    <row r="49" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J49" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+    </row>
+    <row r="50" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J50" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>